<commit_message>
spark by samples examples.
</commit_message>
<xml_diff>
--- a/BigData/TopicListAndBacklog.xlsx
+++ b/BigData/TopicListAndBacklog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\GitHub\DataEngineering\BigData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FA43ED7-8F3E-4F31-9F9F-ADAF184BD216}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B75312AF-A36E-4340-B751-AB49E240A162}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{9D57FCBF-5F65-4056-9614-C69B45A4A813}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="33">
   <si>
     <t>#</t>
   </si>
@@ -516,8 +516,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CC6AC80-BDE9-4C48-A6E3-B14F4136D31F}">
   <dimension ref="B1:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -573,6 +573,9 @@
       </c>
       <c r="F5" s="1" t="s">
         <v>7</v>
+      </c>
+      <c r="G5" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
adding all changes. yet to review
</commit_message>
<xml_diff>
--- a/BigData/TopicListAndBacklog.xlsx
+++ b/BigData/TopicListAndBacklog.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\GitHub\DataEngineering\BigData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B75312AF-A36E-4340-B751-AB49E240A162}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A54F924-33B5-45AF-A313-8AE05A2987ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{9D57FCBF-5F65-4056-9614-C69B45A4A813}"/>
   </bookViews>
@@ -517,7 +517,7 @@
   <dimension ref="B1:G29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="E8" sqref="E8:G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>